<commit_message>
Added nucleic_acid_source field to optimus sheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_optimus_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_optimus_10X_bundle.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengche/Mint/CodePlayground/Playground/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD270B0-39C9-CD4B-89E9-012363CF8374}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="993" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31880" windowHeight="17640" tabRatio="993" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="Library preparation protocol" sheetId="9" r:id="rId10"/>
     <sheet name="Sequencing protocol" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="702">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2140,12 +2141,18 @@
   </si>
   <si>
     <t>pbmc4k_200k_S1_L001_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.nucleic_acid_source</t>
+  </si>
+  <si>
+    <t>single cell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2622,7 +2629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2842,7 +2849,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="6" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>696</v>
       </c>
@@ -2896,16 +2903,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:AU5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>464</v>
       </c>
@@ -2951,101 +2961,102 @@
       <c r="O1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>390</v>
       </c>
@@ -3092,100 +3103,103 @@
         <v>546</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>478</v>
       </c>
@@ -3201,80 +3215,80 @@
       <c r="I3" t="s">
         <v>558</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>316</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>317</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>318</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>319</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>320</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>321</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>316</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>317</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>318</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>319</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>320</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>321</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>559</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>560</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>561</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>316</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>317</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>318</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>319</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>320</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>321</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>562</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>557</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>457</v>
       </c>
@@ -3320,101 +3334,104 @@
       <c r="O4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AT4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>53</v>
       </c>
@@ -3432,7 +3449,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
@@ -3464,8 +3481,9 @@
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:47" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>672</v>
       </c>
@@ -3502,32 +3520,35 @@
       <c r="O6" s="6" t="s">
         <v>600</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="AB6" s="6" t="s">
+      <c r="P6" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="AC6" s="6" t="s">
         <v>601</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AD6" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AM6" s="7" t="s">
         <v>604</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AN6" s="6">
         <v>0</v>
       </c>
-      <c r="AN6" s="6">
+      <c r="AO6" s="6">
         <v>16</v>
       </c>
-      <c r="AO6" s="6" t="s">
+      <c r="AP6" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="AP6" s="6" t="s">
+      <c r="AQ6" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="AQ6" s="6" t="s">
+      <c r="AR6" s="6" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3538,10 +3559,10 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -3768,7 +3789,7 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>675</v>
       </c>
@@ -3828,7 +3849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3841,7 +3862,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3984,7 +4005,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>97</v>
       </c>
@@ -4018,7 +4039,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4026,7 +4047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -4637,7 +4658,7 @@
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
     </row>
-    <row r="6" spans="1:55" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>654</v>
       </c>
@@ -4778,7 +4799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5288,7 +5309,7 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>660</v>
       </c>
@@ -5366,10 +5387,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
@@ -5766,7 +5787,7 @@
       <c r="AF5" s="12"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>663</v>
       </c>
@@ -5862,10 +5883,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -6020,7 +6041,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>697</v>
       </c>
@@ -6055,7 +6076,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>698</v>
       </c>
@@ -6090,7 +6111,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>699</v>
       </c>
@@ -6146,7 +6167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6348,7 +6369,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>666</v>
       </c>
@@ -6402,7 +6423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6609,7 +6630,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>669</v>
       </c>
@@ -6645,7 +6666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6812,7 +6833,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>678</v>
       </c>

</xml_diff>

<commit_message>
Made accessions in testing files valid with schema change
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_optimus_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_optimus_10X_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshadbolt/Desktop/git_repos/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5DFC94-7607-E84B-BD54-5E2C3409C73A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53609508-D1FF-0B47-A574-5FD27D0CCCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="5960" windowWidth="28800" windowHeight="16580" tabRatio="993" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45920" yWindow="4600" windowWidth="37920" windowHeight="19800" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -2695,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2732,7 +2732,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
@@ -2741,7 +2741,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -2779,7 +2779,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>23</v>
@@ -2788,7 +2788,7 @@
         <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
@@ -2823,7 +2823,7 @@
         <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>37</v>
@@ -2832,7 +2832,7 @@
         <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
         <v>40</v>
@@ -2937,7 +2937,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>37</v>
@@ -2946,7 +2946,7 @@
         <v>38</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>40</v>
@@ -5906,7 +5906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6:K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>